<commit_message>
adding a function to inspect whether transaction is within date range of previous month
</commit_message>
<xml_diff>
--- a/RetailerCustomers.xlsx
+++ b/RetailerCustomers.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/073a2ad6e5228e04/111/dev/appv1/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\!\projects\PycharmProjects\beer\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="43" documentId="11_F25DC773A252ABDACC10485FB1DF51685BDE58EC" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{BF462E02-EBF9-4826-8E6F-785A7424C452}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A88C780-C0DF-4587-BE63-8905809EED9A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7370" yWindow="8070" windowWidth="16570" windowHeight="8950" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="380" yWindow="380" windowWidth="16570" windowHeight="8950" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -399,7 +399,7 @@
   <dimension ref="A1:H3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -470,6 +470,12 @@
       <c r="A3">
         <v>2</v>
       </c>
+      <c r="B3">
+        <v>123456</v>
+      </c>
+      <c r="C3">
+        <v>566666</v>
+      </c>
       <c r="D3" t="s">
         <v>11</v>
       </c>

</xml_diff>